<commit_message>
gen IV now handles double battles for Platinum and HGSS
</commit_message>
<xml_diff>
--- a/Gen IV.xlsx
+++ b/Gen IV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abzb1\Dropbox\Programs\Level-Recurver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BC860A-FE73-40B2-A79B-D2CD49093607}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729B7491-A580-4789-AA9F-31A1EDB1264B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1207" windowWidth="25600" windowHeight="13193" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="trpoke" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="135">
   <si>
     <t>Block 1</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Block 9</t>
   </si>
   <si>
-    <t>Block 10</t>
-  </si>
-  <si>
     <t>Level</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>block 19</t>
   </si>
   <si>
-    <t>block 20</t>
-  </si>
-  <si>
     <t>0ch (AI?)</t>
   </si>
   <si>
@@ -198,9 +192,6 @@
     <t>13H</t>
   </si>
   <si>
-    <t xml:space="preserve">19 blocks, each means 3 characters, need to plus </t>
-  </si>
-  <si>
     <t>17 is rival</t>
   </si>
   <si>
@@ -315,30 +306,12 @@
     <t>Falkner</t>
   </si>
   <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>johto</t>
-  </si>
-  <si>
-    <t>kanto</t>
-  </si>
-  <si>
-    <t>e4</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
     <t>Bruno</t>
   </si>
   <si>
     <t>,</t>
   </si>
   <si>
-    <t>[</t>
-  </si>
-  <si>
     <t>]</t>
   </si>
   <si>
@@ -451,16 +424,34 @@
   </si>
   <si>
     <t>'water'</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>block 0</t>
+  </si>
+  <si>
+    <t>Block 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -828,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -841,28 +832,28 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -870,10 +861,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -881,7 +872,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -889,21 +880,21 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -911,7 +902,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -919,7 +910,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -927,10 +918,11 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C13" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -947,313 +939,313 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B18" si="0">B1&amp;A2&amp;C2&amp;D2&amp;E2</f>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500]</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="0"/>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500],['dark',197,198,215,228,229,248,261,262,274,275,302,318,319,332,342,359,430,434,435,442,452,461,491]</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500],['dark',197,198,215,228,229,248,261,262,274,275,302,318,319,332,342,359,430,434,435,442,452,461,491],['dragon',147,148,149,230,329,330,334,371,372,373,380,381,384,443,444,445,483,484,487,501]</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500],['dark',197,198,215,228,229,248,261,262,274,275,302,318,319,332,342,359,430,434,435,442,452,461,491],['dragon',147,148,149,230,329,330,334,371,372,373,380,381,384,443,444,445,483,484,487,501],['electric',25,26,81,82,100,101,125,135,145,170,171,172,179,180,181,239,243,309,310,311,312,403,404,405,417,462,466,479,503,504,505,506,507]</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500],['dark',197,198,215,228,229,248,261,262,274,275,302,318,319,332,342,359,430,434,435,442,452,461,491],['dragon',147,148,149,230,329,330,334,371,372,373,380,381,384,443,444,445,483,484,487,501],['electric',25,26,81,82,100,101,125,135,145,170,171,172,179,180,181,239,243,309,310,311,312,403,404,405,417,462,466,479,503,504,505,506,507],['fighting',56,57,62,66,67,68,106,107,214,236,237,256,257,286,296,297,307,308,391,392,447,448,453,454,475]</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" t="s">
         <v>100</v>
-      </c>
-      <c r="E6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500],['dark',197,198,215,228,229,248,261,262,274,275,302,318,319,332,342,359,430,434,435,442,452,461,491],['dragon',147,148,149,230,329,330,334,371,372,373,380,381,384,443,444,445,483,484,487,501],['electric',25,26,81,82,100,101,125,135,145,170,171,172,179,180,181,239,243,309,310,311,312,403,404,405,417,462,466,479,503,504,505,506,507],['fighting',56,57,62,66,67,68,106,107,214,236,237,256,257,286,296,297,307,308,391,392,447,448,453,454,475],['fire',4,5,6,37,38,58,59,77,78,126,136,146,155,156,157,218,219,228,229,240,244,250,255,256,257,322,323,324,390,391,392,467,485]</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E7" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500],['dark',197,198,215,228,229,248,261,262,274,275,302,318,319,332,342,359,430,434,435,442,452,461,491],['dragon',147,148,149,230,329,330,334,371,372,373,380,381,384,443,444,445,483,484,487,501],['electric',25,26,81,82,100,101,125,135,145,170,171,172,179,180,181,239,243,309,310,311,312,403,404,405,417,462,466,479,503,504,505,506,507],['fighting',56,57,62,66,67,68,106,107,214,236,237,256,257,286,296,297,307,308,391,392,447,448,453,454,475],['fire',4,5,6,37,38,58,59,77,78,126,136,146,155,156,157,218,219,228,229,240,244,250,255,256,257,322,323,324,390,391,392,467,485],['flying',6,12,16,17,18,21,22,41,42,83,84,85,123,130,142,144,145,146,149,163,164,165,166,169,176,177,178,187,188,189,193,198,207,225,226,227,249,250,267,276,277,278,279,284,291,333,334,357,373,384,396,397,398,414,415,416,425,426,430,441,458,468,469,472,502]</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E8" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500],['dark',197,198,215,228,229,248,261,262,274,275,302,318,319,332,342,359,430,434,435,442,452,461,491],['dragon',147,148,149,230,329,330,334,371,372,373,380,381,384,443,444,445,483,484,487,501],['electric',25,26,81,82,100,101,125,135,145,170,171,172,179,180,181,239,243,309,310,311,312,403,404,405,417,462,466,479,503,504,505,506,507],['fighting',56,57,62,66,67,68,106,107,214,236,237,256,257,286,296,297,307,308,391,392,447,448,453,454,475],['fire',4,5,6,37,38,58,59,77,78,126,136,146,155,156,157,218,219,228,229,240,244,250,255,256,257,322,323,324,390,391,392,467,485],['flying',6,12,16,17,18,21,22,41,42,83,84,85,123,130,142,144,145,146,149,163,164,165,166,169,176,177,178,187,188,189,193,198,207,225,226,227,249,250,267,276,277,278,279,284,291,333,334,357,373,384,396,397,398,414,415,416,425,426,430,441,458,468,469,472,502],['ghost',92,93,94,200,292,302,353,354,355,356,425,426,429,442,477,478,479,487,501,503,504,505,506,507]</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D9" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500],['dark',197,198,215,228,229,248,261,262,274,275,302,318,319,332,342,359,430,434,435,442,452,461,491],['dragon',147,148,149,230,329,330,334,371,372,373,380,381,384,443,444,445,483,484,487,501],['electric',25,26,81,82,100,101,125,135,145,170,171,172,179,180,181,239,243,309,310,311,312,403,404,405,417,462,466,479,503,504,505,506,507],['fighting',56,57,62,66,67,68,106,107,214,236,237,256,257,286,296,297,307,308,391,392,447,448,453,454,475],['fire',4,5,6,37,38,58,59,77,78,126,136,146,155,156,157,218,219,228,229,240,244,250,255,256,257,322,323,324,390,391,392,467,485],['flying',6,12,16,17,18,21,22,41,42,83,84,85,123,130,142,144,145,146,149,163,164,165,166,169,176,177,178,187,188,189,193,198,207,225,226,227,249,250,267,276,277,278,279,284,291,333,334,357,373,384,396,397,398,414,415,416,425,426,430,441,458,468,469,472,502],['ghost',92,93,94,200,292,302,353,354,355,356,425,426,429,442,477,478,479,487,501,503,504,505,506,507],['grass',1,2,3,43,44,45,46,47,69,70,71,102,103,114,152,153,154,182,187,188,189,191,192,251,252,253,254,270,271,272,273,274,275,285,286,315,331,332,345,346,357,387,388,389,406,407,413,420,421,455,459,460,465,470,492,499,500,502]</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D10" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E10" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500],['dark',197,198,215,228,229,248,261,262,274,275,302,318,319,332,342,359,430,434,435,442,452,461,491],['dragon',147,148,149,230,329,330,334,371,372,373,380,381,384,443,444,445,483,484,487,501],['electric',25,26,81,82,100,101,125,135,145,170,171,172,179,180,181,239,243,309,310,311,312,403,404,405,417,462,466,479,503,504,505,506,507],['fighting',56,57,62,66,67,68,106,107,214,236,237,256,257,286,296,297,307,308,391,392,447,448,453,454,475],['fire',4,5,6,37,38,58,59,77,78,126,136,146,155,156,157,218,219,228,229,240,244,250,255,256,257,322,323,324,390,391,392,467,485],['flying',6,12,16,17,18,21,22,41,42,83,84,85,123,130,142,144,145,146,149,163,164,165,166,169,176,177,178,187,188,189,193,198,207,225,226,227,249,250,267,276,277,278,279,284,291,333,334,357,373,384,396,397,398,414,415,416,425,426,430,441,458,468,469,472,502],['ghost',92,93,94,200,292,302,353,354,355,356,425,426,429,442,477,478,479,487,501,503,504,505,506,507],['grass',1,2,3,43,44,45,46,47,69,70,71,102,103,114,152,153,154,182,187,188,189,191,192,251,252,253,254,270,271,272,273,274,275,285,286,315,331,332,345,346,357,387,388,389,406,407,413,420,421,455,459,460,465,470,492,499,500,502],['ground',27,28,31,34,50,51,74,75,76,95,104,105,111,112,194,195,207,208,220,221,231,232,246,247,259,260,290,322,323,328,329,330,339,340,343,344,383,389,423,443,444,445,449,450,464,472,473]</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D11" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E11" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500],['dark',197,198,215,228,229,248,261,262,274,275,302,318,319,332,342,359,430,434,435,442,452,461,491],['dragon',147,148,149,230,329,330,334,371,372,373,380,381,384,443,444,445,483,484,487,501],['electric',25,26,81,82,100,101,125,135,145,170,171,172,179,180,181,239,243,309,310,311,312,403,404,405,417,462,466,479,503,504,505,506,507],['fighting',56,57,62,66,67,68,106,107,214,236,237,256,257,286,296,297,307,308,391,392,447,448,453,454,475],['fire',4,5,6,37,38,58,59,77,78,126,136,146,155,156,157,218,219,228,229,240,244,250,255,256,257,322,323,324,390,391,392,467,485],['flying',6,12,16,17,18,21,22,41,42,83,84,85,123,130,142,144,145,146,149,163,164,165,166,169,176,177,178,187,188,189,193,198,207,225,226,227,249,250,267,276,277,278,279,284,291,333,334,357,373,384,396,397,398,414,415,416,425,426,430,441,458,468,469,472,502],['ghost',92,93,94,200,292,302,353,354,355,356,425,426,429,442,477,478,479,487,501,503,504,505,506,507],['grass',1,2,3,43,44,45,46,47,69,70,71,102,103,114,152,153,154,182,187,188,189,191,192,251,252,253,254,270,271,272,273,274,275,285,286,315,331,332,345,346,357,387,388,389,406,407,413,420,421,455,459,460,465,470,492,499,500,502],['ground',27,28,31,34,50,51,74,75,76,95,104,105,111,112,194,195,207,208,220,221,231,232,246,247,259,260,290,322,323,328,329,330,339,340,343,344,383,389,423,443,444,445,449,450,464,472,473],['ice',87,91,124,131,144,215,220,221,225,238,361,362,363,364,365,378,459,460,461,471,473,478]</v>
       </c>
       <c r="C12" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D12" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E12" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500],['dark',197,198,215,228,229,248,261,262,274,275,302,318,319,332,342,359,430,434,435,442,452,461,491],['dragon',147,148,149,230,329,330,334,371,372,373,380,381,384,443,444,445,483,484,487,501],['electric',25,26,81,82,100,101,125,135,145,170,171,172,179,180,181,239,243,309,310,311,312,403,404,405,417,462,466,479,503,504,505,506,507],['fighting',56,57,62,66,67,68,106,107,214,236,237,256,257,286,296,297,307,308,391,392,447,448,453,454,475],['fire',4,5,6,37,38,58,59,77,78,126,136,146,155,156,157,218,219,228,229,240,244,250,255,256,257,322,323,324,390,391,392,467,485],['flying',6,12,16,17,18,21,22,41,42,83,84,85,123,130,142,144,145,146,149,163,164,165,166,169,176,177,178,187,188,189,193,198,207,225,226,227,249,250,267,276,277,278,279,284,291,333,334,357,373,384,396,397,398,414,415,416,425,426,430,441,458,468,469,472,502],['ghost',92,93,94,200,292,302,353,354,355,356,425,426,429,442,477,478,479,487,501,503,504,505,506,507],['grass',1,2,3,43,44,45,46,47,69,70,71,102,103,114,152,153,154,182,187,188,189,191,192,251,252,253,254,270,271,272,273,274,275,285,286,315,331,332,345,346,357,387,388,389,406,407,413,420,421,455,459,460,465,470,492,499,500,502],['ground',27,28,31,34,50,51,74,75,76,95,104,105,111,112,194,195,207,208,220,221,231,232,246,247,259,260,290,322,323,328,329,330,339,340,343,344,383,389,423,443,444,445,449,450,464,472,473],['ice',87,91,124,131,144,215,220,221,225,238,361,362,363,364,365,378,459,460,461,471,473,478],['normal',16,17,18,19,20,21,22,39,40,52,53,83,84,85,108,113,115,128,132,133,137,143,161,162,163,164,174,190,203,206,216,217,233,234,235,241,242,263,264,276,277,287,288,289,293,294,295,298,300,301,327,333,335,351,352,396,397,398,399,400,424,427,428,431,432,440,441,446,463,474,486,493]</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D13" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E13" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500],['dark',197,198,215,228,229,248,261,262,274,275,302,318,319,332,342,359,430,434,435,442,452,461,491],['dragon',147,148,149,230,329,330,334,371,372,373,380,381,384,443,444,445,483,484,487,501],['electric',25,26,81,82,100,101,125,135,145,170,171,172,179,180,181,239,243,309,310,311,312,403,404,405,417,462,466,479,503,504,505,506,507],['fighting',56,57,62,66,67,68,106,107,214,236,237,256,257,286,296,297,307,308,391,392,447,448,453,454,475],['fire',4,5,6,37,38,58,59,77,78,126,136,146,155,156,157,218,219,228,229,240,244,250,255,256,257,322,323,324,390,391,392,467,485],['flying',6,12,16,17,18,21,22,41,42,83,84,85,123,130,142,144,145,146,149,163,164,165,166,169,176,177,178,187,188,189,193,198,207,225,226,227,249,250,267,276,277,278,279,284,291,333,334,357,373,384,396,397,398,414,415,416,425,426,430,441,458,468,469,472,502],['ghost',92,93,94,200,292,302,353,354,355,356,425,426,429,442,477,478,479,487,501,503,504,505,506,507],['grass',1,2,3,43,44,45,46,47,69,70,71,102,103,114,152,153,154,182,187,188,189,191,192,251,252,253,254,270,271,272,273,274,275,285,286,315,331,332,345,346,357,387,388,389,406,407,413,420,421,455,459,460,465,470,492,499,500,502],['ground',27,28,31,34,50,51,74,75,76,95,104,105,111,112,194,195,207,208,220,221,231,232,246,247,259,260,290,322,323,328,329,330,339,340,343,344,383,389,423,443,444,445,449,450,464,472,473],['ice',87,91,124,131,144,215,220,221,225,238,361,362,363,364,365,378,459,460,461,471,473,478],['normal',16,17,18,19,20,21,22,39,40,52,53,83,84,85,108,113,115,128,132,133,137,143,161,162,163,164,174,190,203,206,216,217,233,234,235,241,242,263,264,276,277,287,288,289,293,294,295,298,300,301,327,333,335,351,352,396,397,398,399,400,424,427,428,431,432,440,441,446,463,474,486,493],['poison',1,2,3,13,14,15,23,24,29,30,31,32,33,34,41,42,43,44,45,48,49,69,70,71,72,73,88,89,92,93,94,109,110,167,168,169,211,269,315,316,317,336,406,407,434,435,451,452,453,454]</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D14" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E14" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500],['dark',197,198,215,228,229,248,261,262,274,275,302,318,319,332,342,359,430,434,435,442,452,461,491],['dragon',147,148,149,230,329,330,334,371,372,373,380,381,384,443,444,445,483,484,487,501],['electric',25,26,81,82,100,101,125,135,145,170,171,172,179,180,181,239,243,309,310,311,312,403,404,405,417,462,466,479,503,504,505,506,507],['fighting',56,57,62,66,67,68,106,107,214,236,237,256,257,286,296,297,307,308,391,392,447,448,453,454,475],['fire',4,5,6,37,38,58,59,77,78,126,136,146,155,156,157,218,219,228,229,240,244,250,255,256,257,322,323,324,390,391,392,467,485],['flying',6,12,16,17,18,21,22,41,42,83,84,85,123,130,142,144,145,146,149,163,164,165,166,169,176,177,178,187,188,189,193,198,207,225,226,227,249,250,267,276,277,278,279,284,291,333,334,357,373,384,396,397,398,414,415,416,425,426,430,441,458,468,469,472,502],['ghost',92,93,94,200,292,302,353,354,355,356,425,426,429,442,477,478,479,487,501,503,504,505,506,507],['grass',1,2,3,43,44,45,46,47,69,70,71,102,103,114,152,153,154,182,187,188,189,191,192,251,252,253,254,270,271,272,273,274,275,285,286,315,331,332,345,346,357,387,388,389,406,407,413,420,421,455,459,460,465,470,492,499,500,502],['ground',27,28,31,34,50,51,74,75,76,95,104,105,111,112,194,195,207,208,220,221,231,232,246,247,259,260,290,322,323,328,329,330,339,340,343,344,383,389,423,443,444,445,449,450,464,472,473],['ice',87,91,124,131,144,215,220,221,225,238,361,362,363,364,365,378,459,460,461,471,473,478],['normal',16,17,18,19,20,21,22,39,40,52,53,83,84,85,108,113,115,128,132,133,137,143,161,162,163,164,174,190,203,206,216,217,233,234,235,241,242,263,264,276,277,287,288,289,293,294,295,298,300,301,327,333,335,351,352,396,397,398,399,400,424,427,428,431,432,440,441,446,463,474,486,493],['poison',1,2,3,13,14,15,23,24,29,30,31,32,33,34,41,42,43,44,45,48,49,69,70,71,72,73,88,89,92,93,94,109,110,167,168,169,211,269,315,316,317,336,406,407,434,435,451,452,453,454],['psychic',63,64,65,79,80,96,97,102,103,121,122,124,150,151,177,178,196,199,201,202,203,238,249,251,280,281,282,307,308,325,326,337,338,343,344,358,360,374,375,376,380,381,385,386,433,436,437,439,475,480,481,482,488,496,497,498]</v>
       </c>
       <c r="C15" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D15" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500],['dark',197,198,215,228,229,248,261,262,274,275,302,318,319,332,342,359,430,434,435,442,452,461,491],['dragon',147,148,149,230,329,330,334,371,372,373,380,381,384,443,444,445,483,484,487,501],['electric',25,26,81,82,100,101,125,135,145,170,171,172,179,180,181,239,243,309,310,311,312,403,404,405,417,462,466,479,503,504,505,506,507],['fighting',56,57,62,66,67,68,106,107,214,236,237,256,257,286,296,297,307,308,391,392,447,448,453,454,475],['fire',4,5,6,37,38,58,59,77,78,126,136,146,155,156,157,218,219,228,229,240,244,250,255,256,257,322,323,324,390,391,392,467,485],['flying',6,12,16,17,18,21,22,41,42,83,84,85,123,130,142,144,145,146,149,163,164,165,166,169,176,177,178,187,188,189,193,198,207,225,226,227,249,250,267,276,277,278,279,284,291,333,334,357,373,384,396,397,398,414,415,416,425,426,430,441,458,468,469,472,502],['ghost',92,93,94,200,292,302,353,354,355,356,425,426,429,442,477,478,479,487,501,503,504,505,506,507],['grass',1,2,3,43,44,45,46,47,69,70,71,102,103,114,152,153,154,182,187,188,189,191,192,251,252,253,254,270,271,272,273,274,275,285,286,315,331,332,345,346,357,387,388,389,406,407,413,420,421,455,459,460,465,470,492,499,500,502],['ground',27,28,31,34,50,51,74,75,76,95,104,105,111,112,194,195,207,208,220,221,231,232,246,247,259,260,290,322,323,328,329,330,339,340,343,344,383,389,423,443,444,445,449,450,464,472,473],['ice',87,91,124,131,144,215,220,221,225,238,361,362,363,364,365,378,459,460,461,471,473,478],['normal',16,17,18,19,20,21,22,39,40,52,53,83,84,85,108,113,115,128,132,133,137,143,161,162,163,164,174,190,203,206,216,217,233,234,235,241,242,263,264,276,277,287,288,289,293,294,295,298,300,301,327,333,335,351,352,396,397,398,399,400,424,427,428,431,432,440,441,446,463,474,486,493],['poison',1,2,3,13,14,15,23,24,29,30,31,32,33,34,41,42,43,44,45,48,49,69,70,71,72,73,88,89,92,93,94,109,110,167,168,169,211,269,315,316,317,336,406,407,434,435,451,452,453,454],['psychic',63,64,65,79,80,96,97,102,103,121,122,124,150,151,177,178,196,199,201,202,203,238,249,251,280,281,282,307,308,325,326,337,338,343,344,358,360,374,375,376,380,381,385,386,433,436,437,439,475,480,481,482,488,496,497,498],['rock',74,75,76,95,111,112,138,139,140,141,142,185,213,219,222,246,247,248,299,304,305,306,337,338,345,346,347,348,369,377,408,409,410,411,438,464,476]</v>
       </c>
       <c r="C16" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D16" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E16" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500],['dark',197,198,215,228,229,248,261,262,274,275,302,318,319,332,342,359,430,434,435,442,452,461,491],['dragon',147,148,149,230,329,330,334,371,372,373,380,381,384,443,444,445,483,484,487,501],['electric',25,26,81,82,100,101,125,135,145,170,171,172,179,180,181,239,243,309,310,311,312,403,404,405,417,462,466,479,503,504,505,506,507],['fighting',56,57,62,66,67,68,106,107,214,236,237,256,257,286,296,297,307,308,391,392,447,448,453,454,475],['fire',4,5,6,37,38,58,59,77,78,126,136,146,155,156,157,218,219,228,229,240,244,250,255,256,257,322,323,324,390,391,392,467,485],['flying',6,12,16,17,18,21,22,41,42,83,84,85,123,130,142,144,145,146,149,163,164,165,166,169,176,177,178,187,188,189,193,198,207,225,226,227,249,250,267,276,277,278,279,284,291,333,334,357,373,384,396,397,398,414,415,416,425,426,430,441,458,468,469,472,502],['ghost',92,93,94,200,292,302,353,354,355,356,425,426,429,442,477,478,479,487,501,503,504,505,506,507],['grass',1,2,3,43,44,45,46,47,69,70,71,102,103,114,152,153,154,182,187,188,189,191,192,251,252,253,254,270,271,272,273,274,275,285,286,315,331,332,345,346,357,387,388,389,406,407,413,420,421,455,459,460,465,470,492,499,500,502],['ground',27,28,31,34,50,51,74,75,76,95,104,105,111,112,194,195,207,208,220,221,231,232,246,247,259,260,290,322,323,328,329,330,339,340,343,344,383,389,423,443,444,445,449,450,464,472,473],['ice',87,91,124,131,144,215,220,221,225,238,361,362,363,364,365,378,459,460,461,471,473,478],['normal',16,17,18,19,20,21,22,39,40,52,53,83,84,85,108,113,115,128,132,133,137,143,161,162,163,164,174,190,203,206,216,217,233,234,235,241,242,263,264,276,277,287,288,289,293,294,295,298,300,301,327,333,335,351,352,396,397,398,399,400,424,427,428,431,432,440,441,446,463,474,486,493],['poison',1,2,3,13,14,15,23,24,29,30,31,32,33,34,41,42,43,44,45,48,49,69,70,71,72,73,88,89,92,93,94,109,110,167,168,169,211,269,315,316,317,336,406,407,434,435,451,452,453,454],['psychic',63,64,65,79,80,96,97,102,103,121,122,124,150,151,177,178,196,199,201,202,203,238,249,251,280,281,282,307,308,325,326,337,338,343,344,358,360,374,375,376,380,381,385,386,433,436,437,439,475,480,481,482,488,496,497,498],['rock',74,75,76,95,111,112,138,139,140,141,142,185,213,219,222,246,247,248,299,304,305,306,337,338,345,346,347,348,369,377,408,409,410,411,438,464,476],['steel',81,82,205,208,212,227,303,304,305,306,374,375,376,379,385,395,410,411,436,437,448,462,476,483,485]</v>
       </c>
       <c r="C17" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D17" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E17" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>[['bug',10,11,12,13,14,15,46,47,48,49,123,127,165,166,167,168,193,204,205,212,213,214,265,266,267,268,269,283,284,290,291,292,313,314,347,348,401,402,412,413,414,415,416,451,469,499,500],['dark',197,198,215,228,229,248,261,262,274,275,302,318,319,332,342,359,430,434,435,442,452,461,491],['dragon',147,148,149,230,329,330,334,371,372,373,380,381,384,443,444,445,483,484,487,501],['electric',25,26,81,82,100,101,125,135,145,170,171,172,179,180,181,239,243,309,310,311,312,403,404,405,417,462,466,479,503,504,505,506,507],['fighting',56,57,62,66,67,68,106,107,214,236,237,256,257,286,296,297,307,308,391,392,447,448,453,454,475],['fire',4,5,6,37,38,58,59,77,78,126,136,146,155,156,157,218,219,228,229,240,244,250,255,256,257,322,323,324,390,391,392,467,485],['flying',6,12,16,17,18,21,22,41,42,83,84,85,123,130,142,144,145,146,149,163,164,165,166,169,176,177,178,187,188,189,193,198,207,225,226,227,249,250,267,276,277,278,279,284,291,333,334,357,373,384,396,397,398,414,415,416,425,426,430,441,458,468,469,472,502],['ghost',92,93,94,200,292,302,353,354,355,356,425,426,429,442,477,478,479,487,501,503,504,505,506,507],['grass',1,2,3,43,44,45,46,47,69,70,71,102,103,114,152,153,154,182,187,188,189,191,192,251,252,253,254,270,271,272,273,274,275,285,286,315,331,332,345,346,357,387,388,389,406,407,413,420,421,455,459,460,465,470,492,499,500,502],['ground',27,28,31,34,50,51,74,75,76,95,104,105,111,112,194,195,207,208,220,221,231,232,246,247,259,260,290,322,323,328,329,330,339,340,343,344,383,389,423,443,444,445,449,450,464,472,473],['ice',87,91,124,131,144,215,220,221,225,238,361,362,363,364,365,378,459,460,461,471,473,478],['normal',16,17,18,19,20,21,22,39,40,52,53,83,84,85,108,113,115,128,132,133,137,143,161,162,163,164,174,190,203,206,216,217,233,234,235,241,242,263,264,276,277,287,288,289,293,294,295,298,300,301,327,333,335,351,352,396,397,398,399,400,424,427,428,431,432,440,441,446,463,474,486,493],['poison',1,2,3,13,14,15,23,24,29,30,31,32,33,34,41,42,43,44,45,48,49,69,70,71,72,73,88,89,92,93,94,109,110,167,168,169,211,269,315,316,317,336,406,407,434,435,451,452,453,454],['psychic',63,64,65,79,80,96,97,102,103,121,122,124,150,151,177,178,196,199,201,202,203,238,249,251,280,281,282,307,308,325,326,337,338,343,344,358,360,374,375,376,380,381,385,386,433,436,437,439,475,480,481,482,488,496,497,498],['rock',74,75,76,95,111,112,138,139,140,141,142,185,213,219,222,246,247,248,299,304,305,306,337,338,345,346,347,348,369,377,408,409,410,411,438,464,476],['steel',81,82,205,208,212,227,303,304,305,306,374,375,376,379,385,395,410,411,436,437,448,462,476,483,485],['water',7,8,9,54,55,60,61,62,72,73,79,80,86,87,90,91,98,99,116,117,118,119,120,121,129,130,131,134,138,139,140,141,158,159,160,170,171,183,184,186,194,195,199,211,222,223,224,226,230,245,258,259,260,270,271,272,278,279,283,318,319,320,321,339,340,341,342,349,350,363,364,365,366,367,368,369,370,382,393,394,395,400,418,419,422,423,456,457,458,484,489,490]</v>
       </c>
       <c r="C18" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D18" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E18" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B19" t="str">
         <f>B18&amp;A19</f>
@@ -1270,7 +1262,7 @@
   <dimension ref="A1:O772"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C20"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1288,10 +1280,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>133</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K1">
         <v>1</v>
@@ -1313,25 +1305,25 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
         <v>56</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>57</v>
-      </c>
-      <c r="G2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" t="s">
-        <v>60</v>
       </c>
       <c r="K2">
         <f>K1+1</f>
@@ -1355,7 +1347,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K28" si="1">K2+1</f>
@@ -1379,10 +1371,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K4">
         <f t="shared" si="1"/>
@@ -1406,10 +1398,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
@@ -1433,10 +1425,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
@@ -1460,10 +1452,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
@@ -1487,10 +1479,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K8">
         <f t="shared" si="1"/>
@@ -1514,10 +1506,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K9">
         <f t="shared" si="1"/>
@@ -1541,10 +1533,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K10">
         <f t="shared" si="1"/>
@@ -1568,10 +1560,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K11">
         <f t="shared" si="1"/>
@@ -1595,10 +1587,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
@@ -1622,10 +1614,10 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
@@ -1649,10 +1641,10 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
@@ -1676,10 +1668,10 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K15">
         <f t="shared" si="1"/>
@@ -1703,10 +1695,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K16">
         <f t="shared" si="1"/>
@@ -1730,10 +1722,10 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K17">
         <f t="shared" si="1"/>
@@ -1757,10 +1749,10 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K18">
         <f t="shared" si="1"/>
@@ -1784,10 +1776,10 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K19">
         <f t="shared" si="1"/>
@@ -1811,10 +1803,10 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K20">
         <f t="shared" si="1"/>
@@ -1832,7 +1824,7 @@
         <v>42</v>
       </c>
       <c r="O20" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.5">
@@ -1852,17 +1844,10 @@
         <v>43</v>
       </c>
       <c r="O21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="D22" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22">
-        <f>19*3</f>
-        <v>57</v>
-      </c>
       <c r="K22">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1991,7 +1976,7 @@
         <v>46</v>
       </c>
       <c r="O30" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.5">
@@ -2011,7 +1996,7 @@
         <v>48</v>
       </c>
       <c r="O31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.5">
@@ -2031,7 +2016,7 @@
         <v>49</v>
       </c>
       <c r="O32" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="11:15" x14ac:dyDescent="0.5">
@@ -2048,10 +2033,10 @@
         <v>280</v>
       </c>
       <c r="N33" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="O33" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="11:15" x14ac:dyDescent="0.5">
@@ -2068,10 +2053,10 @@
         <v>294</v>
       </c>
       <c r="N34" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="O34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="11:15" x14ac:dyDescent="0.5">
@@ -2088,10 +2073,10 @@
         <v>2A8</v>
       </c>
       <c r="N35" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O35" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="11:15" x14ac:dyDescent="0.5">
@@ -5023,7 +5008,7 @@
         <v>56</v>
       </c>
       <c r="O244" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="245" spans="11:15" x14ac:dyDescent="0.5">
@@ -5043,7 +5028,7 @@
         <v>57</v>
       </c>
       <c r="O245" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="246" spans="11:15" x14ac:dyDescent="0.5">
@@ -5063,7 +5048,7 @@
         <v>58</v>
       </c>
       <c r="O246" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="247" spans="11:15" x14ac:dyDescent="0.5">
@@ -5083,7 +5068,7 @@
         <v>59</v>
       </c>
       <c r="O247" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="248" spans="11:15" x14ac:dyDescent="0.5">
@@ -5173,7 +5158,7 @@
         <v>62</v>
       </c>
       <c r="O253" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="254" spans="11:15" x14ac:dyDescent="0.5">
@@ -5193,7 +5178,7 @@
         <v>67</v>
       </c>
       <c r="O254" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="255" spans="11:15" x14ac:dyDescent="0.5">
@@ -5213,7 +5198,7 @@
         <v>68</v>
       </c>
       <c r="O255" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="256" spans="11:15" x14ac:dyDescent="0.5">
@@ -5233,7 +5218,7 @@
         <v>69</v>
       </c>
       <c r="O256" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="257" spans="9:15" x14ac:dyDescent="0.5">
@@ -5250,10 +5235,10 @@
         <v>1400</v>
       </c>
       <c r="N257" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="O257" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="258" spans="9:15" x14ac:dyDescent="0.5">
@@ -5270,10 +5255,10 @@
         <v>1414</v>
       </c>
       <c r="N258" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="O258" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="259" spans="9:15" x14ac:dyDescent="0.5">
@@ -5290,15 +5275,15 @@
         <v>1428</v>
       </c>
       <c r="N259" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="O259" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="260" spans="9:15" x14ac:dyDescent="0.5">
       <c r="I260" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J260">
         <v>1</v>
@@ -12485,578 +12470,902 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
         <v>61</v>
       </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" t="s">
-        <v>95</v>
-      </c>
       <c r="G1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>63</v>
-      </c>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B2">
-        <f t="shared" ref="B2:B24" si="0">HEX2DEC(C2)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" t="str">
+        <f>_xlfn.CONCAT(G1,B2,H2)</f>
+        <v>{0,</v>
+      </c>
+      <c r="H2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="str">
+        <f>_xlfn.CONCAT(G2,B3,H3)</f>
+        <v>{0,1,</v>
+      </c>
+      <c r="H3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <f>HEX2DEC(C4)</f>
         <v>23</v>
       </c>
-      <c r="C2">
+      <c r="C4">
         <v>17</v>
       </c>
-      <c r="D2">
+      <c r="D4">
         <v>0</v>
       </c>
-      <c r="E2">
-        <f>COUNT(D:D)</f>
-        <v>23</v>
-      </c>
-      <c r="F2">
-        <f>COUNTIFS(D:D,"&lt;20",D:D,"&gt;10")</f>
-        <v>8</v>
-      </c>
-      <c r="G2">
-        <f>COUNTIFS(D:D,"&lt;40",D:D,"&gt;30")</f>
-        <v>8</v>
-      </c>
-      <c r="H2">
-        <f>COUNTIFS(D:D,"&lt;30",D:D,"&gt;20")</f>
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <f>COUNTIFS(D:D,"&lt;50",D:D,"&gt;39")</f>
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L2" t="str">
-        <f t="shared" ref="L2:L24" si="1">L1&amp;B2&amp;K2</f>
-        <v>[23,</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3">
+      <c r="G4" t="str">
+        <f t="shared" ref="G4:G54" si="0">_xlfn.CONCAT(G3,B4,H4)</f>
+        <v>{0,1,23,</v>
+      </c>
+      <c r="H4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B5">
+        <v>26</v>
+      </c>
+      <c r="G5" t="str">
         <f t="shared" si="0"/>
+        <v>{0,1,23,26,</v>
+      </c>
+      <c r="H5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B6">
+        <v>27</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,</v>
+      </c>
+      <c r="H6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B7">
+        <v>47</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,</v>
+      </c>
+      <c r="H7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ref="B8:B19" si="1">HEX2DEC(C8)</f>
         <v>66</v>
       </c>
-      <c r="C3">
+      <c r="C8">
         <v>42</v>
       </c>
-      <c r="D3">
+      <c r="D8">
         <v>11</v>
       </c>
-      <c r="K3" t="s">
-        <v>100</v>
-      </c>
-      <c r="L3" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A4" t="s">
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,</v>
+      </c>
+      <c r="H8" t="s">
         <v>92</v>
       </c>
-      <c r="B4">
-        <f t="shared" si="0"/>
-        <v>67</v>
-      </c>
-      <c r="C4">
-        <v>43</v>
-      </c>
-      <c r="D4">
-        <v>12</v>
-      </c>
-      <c r="K4" t="s">
-        <v>100</v>
-      </c>
-      <c r="L4" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="C5">
-        <v>46</v>
-      </c>
-      <c r="D5">
-        <v>13</v>
-      </c>
-      <c r="K5" t="s">
-        <v>100</v>
-      </c>
-      <c r="L5" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="C6">
-        <v>48</v>
-      </c>
-      <c r="D6">
-        <v>14</v>
-      </c>
-      <c r="K6" t="s">
-        <v>100</v>
-      </c>
-      <c r="L6" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="C7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7">
-        <v>15</v>
-      </c>
-      <c r="K7" t="s">
-        <v>100</v>
-      </c>
-      <c r="L7" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-      <c r="C8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8">
-        <v>16</v>
-      </c>
-      <c r="K8" t="s">
-        <v>100</v>
-      </c>
-      <c r="L8" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>89</v>
       </c>
       <c r="B9">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="C9">
+        <v>43</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="G9" t="str">
         <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,</v>
+      </c>
+      <c r="H9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="C10">
+        <v>46</v>
+      </c>
+      <c r="D10">
+        <v>13</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,</v>
+      </c>
+      <c r="H10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="C11">
+        <v>48</v>
+      </c>
+      <c r="D11">
+        <v>14</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,</v>
+      </c>
+      <c r="H11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="C9">
+      <c r="C12">
         <v>49</v>
       </c>
-      <c r="D9">
+      <c r="D12">
         <v>17</v>
       </c>
-      <c r="K9" t="s">
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,</v>
+      </c>
+      <c r="H12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13">
+        <v>16</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,</v>
+      </c>
+      <c r="H13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14">
+        <v>15</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,</v>
+      </c>
+      <c r="H14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15">
+        <v>18</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,</v>
+      </c>
+      <c r="H15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="C16">
+        <v>56</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,</v>
+      </c>
+      <c r="H16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="C17">
+        <v>57</v>
+      </c>
+      <c r="D17">
+        <v>21</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,</v>
+      </c>
+      <c r="H17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="C18">
+        <v>58</v>
+      </c>
+      <c r="D18">
+        <v>24</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,</v>
+      </c>
+      <c r="H18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="C19">
+        <v>59</v>
+      </c>
+      <c r="D19">
+        <v>23</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,</v>
+      </c>
+      <c r="H19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B20">
+        <v>90</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,</v>
+      </c>
+      <c r="H20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B21">
+        <v>91</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,</v>
+      </c>
+      <c r="H21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B22">
+        <v>92</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,</v>
+      </c>
+      <c r="H22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B23">
+        <v>93</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,</v>
+      </c>
+      <c r="H23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B24">
+        <v>94</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,</v>
+      </c>
+      <c r="H24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B25">
+        <v>95</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,</v>
+      </c>
+      <c r="H25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B26">
+        <v>96</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,</v>
+      </c>
+      <c r="H26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B27">
+        <v>97</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,</v>
+      </c>
+      <c r="H27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28">
+        <f>HEX2DEC(C28)</f>
+        <v>98</v>
+      </c>
+      <c r="C28">
+        <v>62</v>
+      </c>
+      <c r="D28">
+        <v>31</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,</v>
+      </c>
+      <c r="H28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B29">
+        <v>99</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,</v>
+      </c>
+      <c r="H29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B30">
         <v>100</v>
       </c>
-      <c r="L9" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,73,</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10">
+      <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>76</v>
-      </c>
-      <c r="C10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10">
-        <v>18</v>
-      </c>
-      <c r="K10" t="s">
-        <v>100</v>
-      </c>
-      <c r="L10" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,73,76,</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11">
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,</v>
+      </c>
+      <c r="H30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B31">
+        <v>101</v>
+      </c>
+      <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>87</v>
-      </c>
-      <c r="C11">
-        <v>57</v>
-      </c>
-      <c r="D11">
-        <v>21</v>
-      </c>
-      <c r="K11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L11" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,73,76,87,</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12">
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,</v>
+      </c>
+      <c r="H31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B32">
+        <v>102</v>
+      </c>
+      <c r="G32" t="str">
         <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,</v>
+      </c>
+      <c r="H32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ref="B33:B40" si="2">HEX2DEC(C33)</f>
+        <v>103</v>
+      </c>
+      <c r="C33">
+        <v>67</v>
+      </c>
+      <c r="D33">
+        <v>32</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,</v>
+      </c>
+      <c r="H33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="2"/>
+        <v>104</v>
+      </c>
+      <c r="C34">
+        <v>68</v>
+      </c>
+      <c r="D34">
+        <v>33</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,</v>
+      </c>
+      <c r="H34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+      <c r="C35">
+        <v>69</v>
+      </c>
+      <c r="D35">
+        <v>34</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,</v>
+      </c>
+      <c r="H35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="2"/>
+        <v>106</v>
+      </c>
+      <c r="C36" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36">
+        <v>36</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,</v>
+      </c>
+      <c r="H36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="2"/>
+        <v>107</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37">
+        <v>35</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,</v>
+      </c>
+      <c r="H37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+      <c r="C38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38">
+        <v>37</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,</v>
+      </c>
+      <c r="H38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="2"/>
+        <v>109</v>
+      </c>
+      <c r="C39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39">
+        <v>40</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,109,</v>
+      </c>
+      <c r="H39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="C40" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40">
+        <v>38</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,109,110,</v>
+      </c>
+      <c r="H40" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B41">
+        <v>111</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,109,110,111,</v>
+      </c>
+      <c r="H41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42">
+        <f>HEX2DEC(C42)</f>
         <v>112</v>
       </c>
-      <c r="C12">
+      <c r="C42">
         <v>70</v>
       </c>
-      <c r="D12">
+      <c r="D42">
         <v>22</v>
       </c>
-      <c r="K12" t="s">
-        <v>100</v>
-      </c>
-      <c r="L12" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,73,76,87,112,</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13">
+      <c r="G42" t="str">
         <f t="shared" si="0"/>
-        <v>89</v>
-      </c>
-      <c r="C13">
-        <v>59</v>
-      </c>
-      <c r="D13">
-        <v>23</v>
-      </c>
-      <c r="K13" t="s">
-        <v>100</v>
-      </c>
-      <c r="L13" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,73,76,87,112,89,</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14">
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,109,110,111,112,</v>
+      </c>
+      <c r="H42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B43">
+        <v>113</v>
+      </c>
+      <c r="G43" t="str">
         <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="C14">
-        <v>58</v>
-      </c>
-      <c r="D14">
-        <v>24</v>
-      </c>
-      <c r="K14" t="s">
-        <v>100</v>
-      </c>
-      <c r="L14" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,73,76,87,112,89,88,</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15">
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,109,110,111,112,113,</v>
+      </c>
+      <c r="H43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B44">
+        <v>114</v>
+      </c>
+      <c r="G44" t="str">
         <f t="shared" si="0"/>
-        <v>86</v>
-      </c>
-      <c r="C15">
-        <v>56</v>
-      </c>
-      <c r="D15">
-        <v>25</v>
-      </c>
-      <c r="K15" t="s">
-        <v>100</v>
-      </c>
-      <c r="L15" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,73,76,87,112,89,88,86,</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16">
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,109,110,111,112,113,114,</v>
+      </c>
+      <c r="H44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B45">
+        <v>115</v>
+      </c>
+      <c r="G45" t="str">
         <f t="shared" si="0"/>
-        <v>98</v>
-      </c>
-      <c r="C16">
-        <v>62</v>
-      </c>
-      <c r="D16">
-        <v>31</v>
-      </c>
-      <c r="K16" t="s">
-        <v>100</v>
-      </c>
-      <c r="L16" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,73,76,87,112,89,88,86,98,</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17">
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,109,110,111,112,113,114,115,</v>
+      </c>
+      <c r="H45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B46">
+        <v>116</v>
+      </c>
+      <c r="G46" t="str">
         <f t="shared" si="0"/>
-        <v>103</v>
-      </c>
-      <c r="C17">
-        <v>67</v>
-      </c>
-      <c r="D17">
-        <v>32</v>
-      </c>
-      <c r="K17" t="s">
-        <v>100</v>
-      </c>
-      <c r="L17" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,73,76,87,112,89,88,86,98,103,</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18">
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,109,110,111,112,113,114,115,116,</v>
+      </c>
+      <c r="H46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B47">
+        <v>117</v>
+      </c>
+      <c r="G47" t="str">
         <f t="shared" si="0"/>
-        <v>104</v>
-      </c>
-      <c r="C18">
-        <v>68</v>
-      </c>
-      <c r="D18">
-        <v>33</v>
-      </c>
-      <c r="K18" t="s">
-        <v>100</v>
-      </c>
-      <c r="L18" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,73,76,87,112,89,88,86,98,103,104,</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19">
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,109,110,111,112,113,114,115,116,117,</v>
+      </c>
+      <c r="H47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B48">
+        <v>118</v>
+      </c>
+      <c r="G48" t="str">
         <f t="shared" si="0"/>
-        <v>105</v>
-      </c>
-      <c r="C19">
-        <v>69</v>
-      </c>
-      <c r="D19">
-        <v>34</v>
-      </c>
-      <c r="K19" t="s">
-        <v>100</v>
-      </c>
-      <c r="L19" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,73,76,87,112,89,88,86,98,103,104,105,</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20">
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,109,110,111,112,113,114,115,116,117,118,</v>
+      </c>
+      <c r="H48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.5">
+      <c r="B49">
+        <v>123</v>
+      </c>
+      <c r="G49" t="str">
         <f t="shared" si="0"/>
-        <v>107</v>
-      </c>
-      <c r="C20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20">
-        <v>35</v>
-      </c>
-      <c r="K20" t="s">
-        <v>100</v>
-      </c>
-      <c r="L20" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,73,76,87,112,89,88,86,98,103,104,105,107,</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21">
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,109,110,111,112,113,114,115,116,117,118,123,</v>
+      </c>
+      <c r="H49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.5">
+      <c r="B50">
+        <v>124</v>
+      </c>
+      <c r="G50" t="str">
         <f t="shared" si="0"/>
-        <v>106</v>
-      </c>
-      <c r="C21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21">
-        <v>36</v>
-      </c>
-      <c r="K21" t="s">
-        <v>100</v>
-      </c>
-      <c r="L21" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,73,76,87,112,89,88,86,98,103,104,105,107,106,</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22">
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,109,110,111,112,113,114,115,116,117,118,123,124,</v>
+      </c>
+      <c r="H50" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.5">
+      <c r="B51">
+        <v>125</v>
+      </c>
+      <c r="G51" t="str">
         <f t="shared" si="0"/>
-        <v>108</v>
-      </c>
-      <c r="C22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22">
-        <v>37</v>
-      </c>
-      <c r="K22" t="s">
-        <v>100</v>
-      </c>
-      <c r="L22" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,73,76,87,112,89,88,86,98,103,104,105,107,106,108,</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A23" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23">
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,109,110,111,112,113,114,115,116,117,118,123,124,125,</v>
+      </c>
+      <c r="H51" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.5">
+      <c r="B52">
+        <v>126</v>
+      </c>
+      <c r="G52" t="str">
         <f t="shared" si="0"/>
-        <v>110</v>
-      </c>
-      <c r="C23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23">
-        <v>38</v>
-      </c>
-      <c r="K23" t="s">
-        <v>100</v>
-      </c>
-      <c r="L23" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,73,76,87,112,89,88,86,98,103,104,105,107,106,108,110,</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24">
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,109,110,111,112,113,114,115,116,117,118,123,124,125,126,</v>
+      </c>
+      <c r="H52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.5">
+      <c r="B53">
+        <v>127</v>
+      </c>
+      <c r="G53" t="str">
         <f t="shared" si="0"/>
-        <v>109</v>
-      </c>
-      <c r="C24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24">
-        <v>40</v>
-      </c>
-      <c r="K24" t="s">
-        <v>102</v>
-      </c>
-      <c r="L24" t="str">
-        <f t="shared" si="1"/>
-        <v>[23,66,67,70,72,75,74,73,76,87,112,89,88,86,98,103,104,105,107,106,108,110,109]</v>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,109,110,111,112,113,114,115,116,117,118,123,124,125,126,127,</v>
+      </c>
+      <c r="H53" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.5">
+      <c r="B54">
+        <v>128</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="0"/>
+        <v>{0,1,23,26,27,47,66,67,70,72,73,74,75,76,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105,106,107,108,109,110,111,112,113,114,115,116,117,118,123,124,125,126,127,128}</v>
+      </c>
+      <c r="H54" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D24">
-    <sortCondition ref="D2:D24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D42">
+    <sortCondition ref="B2:B42"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>